<commit_message>
feature importance linear model
</commit_message>
<xml_diff>
--- a/experiments/init/results/sbm_modularity_any3_bestparam_byari_individual.xlsx
+++ b/experiments/init/results/sbm_modularity_any3_bestparam_byari_individual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>100_2_0.05_0.001</t>
   </si>
@@ -154,6 +154,9 @@
     <t>100_4_0.30_0.150</t>
   </si>
   <si>
+    <t>150_2_0.10_0.001</t>
+  </si>
+  <si>
     <t>150_3_0.10_0.001</t>
   </si>
   <si>
@@ -182,6 +185,24 @@
   </si>
   <si>
     <t>201_3_0.30_0.100</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.001</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.005</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.010</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.020</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.050</t>
+  </si>
+  <si>
+    <t>200_4_0.10_0.100</t>
   </si>
   <si>
     <t>200_4_0.30_0.100</t>
@@ -620,13 +641,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG26"/>
+  <dimension ref="A1:BN26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:66">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,10 +822,31 @@
       <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="BH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:59">
+    <row r="2" spans="1:66">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>0.9637630729030069</v>
@@ -945,45 +987,66 @@
         <v>0.09738884064937885</v>
       </c>
       <c r="AV2">
+        <v>0.9997333216416557</v>
+      </c>
+      <c r="AW2">
         <v>0.9967952846470951</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>0.975327380663122</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>0.8440329599630847</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>0.2897864963015163</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>0.05122283276722361</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>0.02232763204907105</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <v>0.9909308405237996</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <v>0.6569928610699992</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <v>0.3114300669880454</v>
       </c>
-      <c r="BE2">
+      <c r="BF2">
         <v>0.3295579674177707</v>
       </c>
-      <c r="BF2">
+      <c r="BG2">
+        <v>0.9969165914032172</v>
+      </c>
+      <c r="BH2">
+        <v>0.9441361237575534</v>
+      </c>
+      <c r="BI2">
+        <v>0.6615499477729663</v>
+      </c>
+      <c r="BJ2">
+        <v>0.1615535829676643</v>
+      </c>
+      <c r="BK2">
+        <v>0.03487929122281073</v>
+      </c>
+      <c r="BL2">
+        <v>0.01428342100979789</v>
+      </c>
+      <c r="BM2">
         <v>0.180573136746276</v>
       </c>
-      <c r="BG2">
+      <c r="BN2">
         <v>0.07851135901753734</v>
       </c>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:66">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>0.9094069535352416</v>
@@ -1124,45 +1187,66 @@
         <v>0.1698314685656082</v>
       </c>
       <c r="AV3">
+        <v>0.9997333216416557</v>
+      </c>
+      <c r="AW3">
         <v>0.9922696255373815</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>0.957887583893135</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>0.8889850002097155</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>0.637160165488049</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>0.08655805437008061</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>0.02203578506605368</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>1</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD3">
+      <c r="BE3">
         <v>0.9804879739419493</v>
       </c>
-      <c r="BE3">
+      <c r="BF3">
         <v>0.9950678743951148</v>
       </c>
-      <c r="BF3">
+      <c r="BG3">
+        <v>0.9863886309697759</v>
+      </c>
+      <c r="BH3">
+        <v>0.9306586356799963</v>
+      </c>
+      <c r="BI3">
+        <v>0.8330394420467792</v>
+      </c>
+      <c r="BJ3">
+        <v>0.4874808429108185</v>
+      </c>
+      <c r="BK3">
+        <v>0.058006083766369</v>
+      </c>
+      <c r="BL3">
+        <v>0.01419496698673787</v>
+      </c>
+      <c r="BM3">
         <v>0.920408727075117</v>
       </c>
-      <c r="BG3">
+      <c r="BN3">
         <v>0.1837670113590898</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:66">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>0.9065387393091242</v>
@@ -1303,45 +1387,66 @@
         <v>0.1387363484084348</v>
       </c>
       <c r="AV4">
+        <v>0.9997333216416557</v>
+      </c>
+      <c r="AW4">
         <v>0.9891033371286558</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>0.9438382314181004</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>0.8515456807115711</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>0.550850037546864</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>0.07353498438936895</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>0.01893914588009453</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>1</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD4">
+      <c r="BE4">
         <v>0.77972505925649</v>
       </c>
-      <c r="BE4">
+      <c r="BF4">
         <v>0.9251495648420902</v>
       </c>
-      <c r="BF4">
+      <c r="BG4">
+        <v>0.9731214201969496</v>
+      </c>
+      <c r="BH4">
+        <v>0.9102090202406775</v>
+      </c>
+      <c r="BI4">
+        <v>0.7808354281723168</v>
+      </c>
+      <c r="BJ4">
+        <v>0.3611228911221068</v>
+      </c>
+      <c r="BK4">
+        <v>0.04585470136190287</v>
+      </c>
+      <c r="BL4">
+        <v>0.01145188990612546</v>
+      </c>
+      <c r="BM4">
         <v>0.4206727553459844</v>
       </c>
-      <c r="BG4">
+      <c r="BN4">
         <v>0.1190681821654176</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:66">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>0.9453617996174155</v>
@@ -1482,45 +1587,66 @@
         <v>0.2261887366683209</v>
       </c>
       <c r="AV5">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW5">
         <v>0.9941865006665246</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>0.9727325866770054</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>0.9250543470928778</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>0.7553721781614621</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>0.1182458433010575</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>0.02313304038267702</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>1</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>0.9993999851515227</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <v>0.9872378827463723</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <v>0.9955191172668674</v>
       </c>
-      <c r="BF5">
+      <c r="BG5">
+        <v>0.994646752344113</v>
+      </c>
+      <c r="BH5">
+        <v>0.9625875713947006</v>
+      </c>
+      <c r="BI5">
+        <v>0.9085258472653507</v>
+      </c>
+      <c r="BJ5">
+        <v>0.6804719299471677</v>
+      </c>
+      <c r="BK5">
+        <v>0.0836596804541747</v>
+      </c>
+      <c r="BL5">
+        <v>0.0167874856413665</v>
+      </c>
+      <c r="BM5">
         <v>0.978038795715463</v>
       </c>
-      <c r="BG5">
+      <c r="BN5">
         <v>0.3955129184763343</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:66">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>0.9676905978028074</v>
@@ -1661,45 +1787,66 @@
         <v>0.2172457901845333</v>
       </c>
       <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6">
         <v>0.9961953545403839</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>0.9735370824200688</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>0.8431420241049485</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>0.3070554179324931</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>0.1337530616171959</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>0.06038883884886161</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>1</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>0.7189422104465518</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>0.4021629526073812</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>0.3634425244558295</v>
       </c>
-      <c r="BF6">
+      <c r="BG6">
+        <v>0.9965280742354939</v>
+      </c>
+      <c r="BH6">
+        <v>0.94363459591424</v>
+      </c>
+      <c r="BI6">
+        <v>0.6557856909304134</v>
+      </c>
+      <c r="BJ6">
+        <v>0.1867712167802713</v>
+      </c>
+      <c r="BK6">
+        <v>0.09227686753790049</v>
+      </c>
+      <c r="BL6">
+        <v>0.04372167221789883</v>
+      </c>
+      <c r="BM6">
         <v>0.2313272048852544</v>
       </c>
-      <c r="BG6">
+      <c r="BN6">
         <v>0.2132430041045927</v>
       </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:66">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>0.9641468988847035</v>
@@ -1840,45 +1987,66 @@
         <v>0.3272983050283574</v>
       </c>
       <c r="AV7">
+        <v>1</v>
+      </c>
+      <c r="AW7">
         <v>0.997192646380856</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <v>0.9768850540143603</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>0.9194980535938487</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>0.6440098487822126</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <v>0.2244389383979003</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>0.1372051058684097</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <v>1</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <v>0.9801120934071256</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>0.9938834322166185</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
+        <v>0.9969259282465214</v>
+      </c>
+      <c r="BH7">
+        <v>0.96403549645121</v>
+      </c>
+      <c r="BI7">
+        <v>0.8752216713866423</v>
+      </c>
+      <c r="BJ7">
+        <v>0.4434134851995332</v>
+      </c>
+      <c r="BK7">
+        <v>0.1773603484864924</v>
+      </c>
+      <c r="BL7">
+        <v>0.1211106271230779</v>
+      </c>
+      <c r="BM7">
         <v>0.926508377146511</v>
       </c>
-      <c r="BG7">
+      <c r="BN7">
         <v>0.3404887253506378</v>
       </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:66">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>0.961762753426727</v>
@@ -2019,45 +2187,66 @@
         <v>0.2247177945007964</v>
       </c>
       <c r="AV8">
+        <v>1</v>
+      </c>
+      <c r="AW8">
         <v>0.9959926202419009</v>
       </c>
-      <c r="AW8">
+      <c r="AX8">
         <v>0.9770960449829786</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <v>0.9210501048553625</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <v>0.7118225609943566</v>
       </c>
-      <c r="AZ8">
+      <c r="BA8">
         <v>0.09672990318361752</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>0.02680524950928695</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <v>1</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <v>0.9836558825697428</v>
       </c>
-      <c r="BE8">
+      <c r="BF8">
         <v>0.9947732146684711</v>
       </c>
-      <c r="BF8">
+      <c r="BG8">
+        <v>0.99598266580908</v>
+      </c>
+      <c r="BH8">
+        <v>0.9653112249206492</v>
+      </c>
+      <c r="BI8">
+        <v>0.8945068258727146</v>
+      </c>
+      <c r="BJ8">
+        <v>0.6383223698317224</v>
+      </c>
+      <c r="BK8">
+        <v>0.07106611390483203</v>
+      </c>
+      <c r="BL8">
+        <v>0.01874757386993528</v>
+      </c>
+      <c r="BM8">
         <v>0.958064930220446</v>
       </c>
-      <c r="BG8">
+      <c r="BN8">
         <v>0.5298135121956674</v>
       </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:66">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>0.8830235822542317</v>
@@ -2198,45 +2387,66 @@
         <v>0.1467598541569674</v>
       </c>
       <c r="AV9">
+        <v>0.9997333216416557</v>
+      </c>
+      <c r="AW9">
         <v>0.9735894446555801</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <v>0.8655275101715642</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>0.6346615780936334</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>0.289412998527052</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <v>0.07305522459755492</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>0.02033208021436642</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <v>1</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <v>0.8438370788670063</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>0.5166592260746014</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <v>0.5186884571188352</v>
       </c>
-      <c r="BF9">
+      <c r="BG9">
+        <v>0.9234016706646517</v>
+      </c>
+      <c r="BH9">
+        <v>0.7463103743356317</v>
+      </c>
+      <c r="BI9">
+        <v>0.4195094201676254</v>
+      </c>
+      <c r="BJ9">
+        <v>0.1865276659785612</v>
+      </c>
+      <c r="BK9">
+        <v>0.04842614711368523</v>
+      </c>
+      <c r="BL9">
+        <v>0.01357219024108321</v>
+      </c>
+      <c r="BM9">
         <v>0.3079838478999686</v>
       </c>
-      <c r="BG9">
+      <c r="BN9">
         <v>0.1263802266694816</v>
       </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:66">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>0.9603409202900892</v>
@@ -2377,45 +2587,66 @@
         <v>0.2219378368297626</v>
       </c>
       <c r="AV10">
+        <v>0.9997333216416557</v>
+      </c>
+      <c r="AW10">
         <v>0.9953926347291053</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <v>0.9678874132064453</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <v>0.8030637939369646</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <v>0.2703048208776692</v>
       </c>
-      <c r="AZ10">
+      <c r="BA10">
         <v>0.1404477226817118</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <v>0.06245555812130524</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <v>0.9691999114778638</v>
       </c>
-      <c r="BC10">
+      <c r="BD10">
         <v>0.6592302594979005</v>
       </c>
-      <c r="BD10">
+      <c r="BE10">
         <v>0.3591815411271408</v>
       </c>
-      <c r="BE10">
+      <c r="BF10">
         <v>0.3268349417803487</v>
       </c>
-      <c r="BF10">
+      <c r="BG10">
+        <v>0.995453296308074</v>
+      </c>
+      <c r="BH10">
+        <v>0.930664046932816</v>
+      </c>
+      <c r="BI10">
+        <v>0.5655554148906075</v>
+      </c>
+      <c r="BJ10">
+        <v>0.1635960017673818</v>
+      </c>
+      <c r="BK10">
+        <v>0.1142123123879254</v>
+      </c>
+      <c r="BL10">
+        <v>0.0451716818290927</v>
+      </c>
+      <c r="BM10">
         <v>0.2160070388816388</v>
       </c>
-      <c r="BG10">
+      <c r="BN10">
         <v>0.1964270695697202</v>
       </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:66">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0.9605218902920385</v>
@@ -2556,45 +2787,66 @@
         <v>0.1851455323801507</v>
       </c>
       <c r="AV11">
+        <v>1</v>
+      </c>
+      <c r="AW11">
         <v>0.9955933146819249</v>
       </c>
-      <c r="AW11">
+      <c r="AX11">
         <v>0.9767072036303028</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <v>0.9233022115158341</v>
       </c>
-      <c r="AY11">
+      <c r="AZ11">
         <v>0.7136392851292399</v>
       </c>
-      <c r="AZ11">
+      <c r="BA11">
         <v>0.08856481128261257</v>
       </c>
-      <c r="BA11">
+      <c r="BB11">
         <v>0.02031165098638557</v>
       </c>
-      <c r="BB11">
+      <c r="BC11">
         <v>1</v>
       </c>
-      <c r="BC11">
+      <c r="BD11">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <v>0.980093987766531</v>
       </c>
-      <c r="BE11">
+      <c r="BF11">
         <v>0.9943208013142053</v>
       </c>
-      <c r="BF11">
+      <c r="BG11">
+        <v>0.9959826470295405</v>
+      </c>
+      <c r="BH11">
+        <v>0.9655502890729598</v>
+      </c>
+      <c r="BI11">
+        <v>0.8938965923276447</v>
+      </c>
+      <c r="BJ11">
+        <v>0.6188263894715703</v>
+      </c>
+      <c r="BK11">
+        <v>0.06025379217139843</v>
+      </c>
+      <c r="BL11">
+        <v>0.0150646994717561</v>
+      </c>
+      <c r="BM11">
         <v>0.9543232134600107</v>
       </c>
-      <c r="BG11">
+      <c r="BN11">
         <v>0.2605061086291137</v>
       </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:66">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>0.9683610781712814</v>
@@ -2735,45 +2987,66 @@
         <v>0.1410017233066609</v>
       </c>
       <c r="AV12">
+        <v>1</v>
+      </c>
+      <c r="AW12">
         <v>0.9967932575768645</v>
       </c>
-      <c r="AW12">
+      <c r="AX12">
         <v>0.9762918381704441</v>
       </c>
-      <c r="AX12">
+      <c r="AY12">
         <v>0.883554552655455</v>
       </c>
-      <c r="AY12">
+      <c r="AZ12">
         <v>0.3849971910867198</v>
       </c>
-      <c r="AZ12">
+      <c r="BA12">
         <v>0.0744411263474265</v>
       </c>
-      <c r="BA12">
+      <c r="BB12">
         <v>0.02429722986148657</v>
       </c>
-      <c r="BB12">
+      <c r="BC12">
         <v>1</v>
       </c>
-      <c r="BC12">
+      <c r="BD12">
         <v>0.8655552227661317</v>
       </c>
-      <c r="BD12">
+      <c r="BE12">
         <v>0.5363356921264437</v>
       </c>
-      <c r="BE12">
+      <c r="BF12">
         <v>0.5739264246635893</v>
       </c>
-      <c r="BF12">
+      <c r="BG12">
+        <v>0.9958594791021533</v>
+      </c>
+      <c r="BH12">
+        <v>0.9574916720813305</v>
+      </c>
+      <c r="BI12">
+        <v>0.7165841909956773</v>
+      </c>
+      <c r="BJ12">
+        <v>0.2379056042389926</v>
+      </c>
+      <c r="BK12">
+        <v>0.05239781044722126</v>
+      </c>
+      <c r="BL12">
+        <v>0.01937221272534833</v>
+      </c>
+      <c r="BM12">
         <v>0.3384527085574912</v>
       </c>
-      <c r="BG12">
+      <c r="BN12">
         <v>0.1319519076333838</v>
       </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:66">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>0.949216825037713</v>
@@ -2914,45 +3187,66 @@
         <v>0.245062345566344</v>
       </c>
       <c r="AV13">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW13">
         <v>0.9951858468526599</v>
       </c>
-      <c r="AW13">
+      <c r="AX13">
         <v>0.9715410807631999</v>
       </c>
-      <c r="AX13">
+      <c r="AY13">
         <v>0.9210607815611134</v>
       </c>
-      <c r="AY13">
+      <c r="AZ13">
         <v>0.7494455617048975</v>
       </c>
-      <c r="AZ13">
+      <c r="BA13">
         <v>0.1300840172051062</v>
       </c>
-      <c r="BA13">
+      <c r="BB13">
         <v>0.02282372110935071</v>
       </c>
-      <c r="BB13">
+      <c r="BC13">
         <v>1</v>
       </c>
-      <c r="BC13">
+      <c r="BD13">
         <v>0.9993999851515227</v>
       </c>
-      <c r="BD13">
+      <c r="BE13">
         <v>0.9822638881100805</v>
       </c>
-      <c r="BE13">
+      <c r="BF13">
         <v>0.9938743807647148</v>
       </c>
-      <c r="BF13">
+      <c r="BG13">
+        <v>0.9955846552207513</v>
+      </c>
+      <c r="BH13">
+        <v>0.9606392134056354</v>
+      </c>
+      <c r="BI13">
+        <v>0.9034927436479241</v>
+      </c>
+      <c r="BJ13">
+        <v>0.6902401240804785</v>
+      </c>
+      <c r="BK13">
+        <v>0.08683588040474816</v>
+      </c>
+      <c r="BL13">
+        <v>0.01760479673076406</v>
+      </c>
+      <c r="BM13">
         <v>0.979107867009006</v>
       </c>
-      <c r="BG13">
+      <c r="BN13">
         <v>0.5383034325082374</v>
       </c>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:66">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>0.9428565882580945</v>
@@ -3093,45 +3387,66 @@
         <v>0.3121176245762534</v>
       </c>
       <c r="AV14">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW14">
         <v>0.9951878179543077</v>
       </c>
-      <c r="AW14">
+      <c r="AX14">
         <v>0.9703309684130511</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>0.9179478690958754</v>
       </c>
-      <c r="AY14">
+      <c r="AZ14">
         <v>0.7420216772335751</v>
       </c>
-      <c r="AZ14">
+      <c r="BA14">
         <v>0.1475778592963888</v>
       </c>
-      <c r="BA14">
+      <c r="BB14">
         <v>0.03839463599178881</v>
       </c>
-      <c r="BB14">
+      <c r="BC14">
         <v>1</v>
       </c>
-      <c r="BC14">
+      <c r="BD14">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD14">
+      <c r="BE14">
         <v>0.9797040303288704</v>
       </c>
-      <c r="BE14">
+      <c r="BF14">
         <v>0.9923915466222113</v>
       </c>
-      <c r="BF14">
+      <c r="BG14">
+        <v>0.995452088795534</v>
+      </c>
+      <c r="BH14">
+        <v>0.9612352058413096</v>
+      </c>
+      <c r="BI14">
+        <v>0.8985169263372967</v>
+      </c>
+      <c r="BJ14">
+        <v>0.6856817286886158</v>
+      </c>
+      <c r="BK14">
+        <v>0.119020324869413</v>
+      </c>
+      <c r="BL14">
+        <v>0.03731895820239367</v>
+      </c>
+      <c r="BM14">
         <v>0.9643834371125928</v>
       </c>
-      <c r="BG14">
+      <c r="BN14">
         <v>0.6359514739353305</v>
       </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:66">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>0.9436404747291145</v>
@@ -3272,45 +3587,66 @@
         <v>0.2773174905766692</v>
       </c>
       <c r="AV15">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW15">
         <v>0.9953926347291053</v>
       </c>
-      <c r="AW15">
+      <c r="AX15">
         <v>0.9786752560890684</v>
       </c>
-      <c r="AX15">
+      <c r="AY15">
         <v>0.9349985179829418</v>
       </c>
-      <c r="AY15">
+      <c r="AZ15">
         <v>0.7487171578975156</v>
       </c>
-      <c r="AZ15">
+      <c r="BA15">
         <v>0.1472880956119361</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>0.03858522841043706</v>
       </c>
-      <c r="BB15">
+      <c r="BC15">
         <v>1</v>
       </c>
-      <c r="BC15">
+      <c r="BD15">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD15">
+      <c r="BE15">
         <v>0.9862358477100936</v>
       </c>
-      <c r="BE15">
+      <c r="BF15">
         <v>0.9952175619894361</v>
       </c>
-      <c r="BF15">
+      <c r="BG15">
+        <v>0.9959880791077411</v>
+      </c>
+      <c r="BH15">
+        <v>0.9685238385463478</v>
+      </c>
+      <c r="BI15">
+        <v>0.9072535032001448</v>
+      </c>
+      <c r="BJ15">
+        <v>0.6803528086047463</v>
+      </c>
+      <c r="BK15">
+        <v>0.1105864339642547</v>
+      </c>
+      <c r="BL15">
+        <v>0.03572801447038757</v>
+      </c>
+      <c r="BM15">
         <v>0.9738311238799138</v>
       </c>
-      <c r="BG15">
+      <c r="BN15">
         <v>0.590839628977808</v>
       </c>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="1:66">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>0.9441052994701791</v>
@@ -3451,45 +3787,66 @@
         <v>0.1840801299322515</v>
       </c>
       <c r="AV16">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW16">
         <v>0.9943852095176965</v>
       </c>
-      <c r="AW16">
+      <c r="AX16">
         <v>0.9766970784070343</v>
       </c>
-      <c r="AX16">
+      <c r="AY16">
         <v>0.9289399411668394</v>
       </c>
-      <c r="AY16">
+      <c r="AZ16">
         <v>0.7265787100339577</v>
       </c>
-      <c r="AZ16">
+      <c r="BA16">
         <v>0.1149587032024183</v>
       </c>
-      <c r="BA16">
+      <c r="BB16">
         <v>0.02531831708879961</v>
       </c>
-      <c r="BB16">
+      <c r="BC16">
         <v>1</v>
       </c>
-      <c r="BC16">
+      <c r="BD16">
         <v>0.9993999851515227</v>
       </c>
-      <c r="BD16">
+      <c r="BE16">
         <v>0.9840518756615299</v>
       </c>
-      <c r="BE16">
+      <c r="BF16">
         <v>0.9944717264911884</v>
       </c>
-      <c r="BF16">
+      <c r="BG16">
+        <v>0.9950569671055998</v>
+      </c>
+      <c r="BH16">
+        <v>0.9657608771023063</v>
+      </c>
+      <c r="BI16">
+        <v>0.8971301958407158</v>
+      </c>
+      <c r="BJ16">
+        <v>0.6440467949846129</v>
+      </c>
+      <c r="BK16">
+        <v>0.07923464908684433</v>
+      </c>
+      <c r="BL16">
+        <v>0.01812368752076735</v>
+      </c>
+      <c r="BM16">
         <v>0.9710753948935753</v>
       </c>
-      <c r="BG16">
+      <c r="BN16">
         <v>0.3461382065212954</v>
       </c>
     </row>
-    <row r="17" spans="1:59">
+    <row r="17" spans="1:66">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>0.9441778646617313</v>
@@ -3630,45 +3987,66 @@
         <v>0.2068469121287884</v>
       </c>
       <c r="AV17">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW17">
         <v>0.9937892775828635</v>
       </c>
-      <c r="AW17">
+      <c r="AX17">
         <v>0.9737211969734867</v>
       </c>
-      <c r="AX17">
+      <c r="AY17">
         <v>0.9254652322201221</v>
       </c>
-      <c r="AY17">
+      <c r="AZ17">
         <v>0.7500146941610393</v>
       </c>
-      <c r="AZ17">
+      <c r="BA17">
         <v>0.1135352234575346</v>
       </c>
-      <c r="BA17">
+      <c r="BB17">
         <v>0.02129036749025407</v>
       </c>
-      <c r="BB17">
+      <c r="BC17">
         <v>1</v>
       </c>
-      <c r="BC17">
+      <c r="BD17">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD17">
+      <c r="BE17">
         <v>0.9878318651081368</v>
       </c>
-      <c r="BE17">
+      <c r="BF17">
         <v>0.9950656472904917</v>
       </c>
-      <c r="BF17">
+      <c r="BG17">
+        <v>0.9943774133031127</v>
+      </c>
+      <c r="BH17">
+        <v>0.9620376917075388</v>
+      </c>
+      <c r="BI17">
+        <v>0.9073370992174812</v>
+      </c>
+      <c r="BJ17">
+        <v>0.6725817311980025</v>
+      </c>
+      <c r="BK17">
+        <v>0.07711567251692911</v>
+      </c>
+      <c r="BL17">
+        <v>0.01472129229869013</v>
+      </c>
+      <c r="BM17">
         <v>0.9729173712746263</v>
       </c>
-      <c r="BG17">
+      <c r="BN17">
         <v>0.3663415811102521</v>
       </c>
     </row>
-    <row r="18" spans="1:59">
+    <row r="18" spans="1:66">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B18">
         <v>0.9350907684137644</v>
@@ -3809,45 +4187,66 @@
         <v>0.262873909547799</v>
       </c>
       <c r="AV18">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW18">
         <v>0.9935804913293379</v>
       </c>
-      <c r="AW18">
+      <c r="AX18">
         <v>0.9573391059330423</v>
       </c>
-      <c r="AX18">
+      <c r="AY18">
         <v>0.9020482632212241</v>
       </c>
-      <c r="AY18">
+      <c r="AZ18">
         <v>0.7375525631625863</v>
       </c>
-      <c r="AZ18">
+      <c r="BA18">
         <v>0.1234637171313173</v>
       </c>
-      <c r="BA18">
+      <c r="BB18">
         <v>0.02503454674821367</v>
       </c>
-      <c r="BB18">
+      <c r="BC18">
         <v>1</v>
       </c>
-      <c r="BC18">
+      <c r="BD18">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD18">
+      <c r="BE18">
         <v>0.9846518883110845</v>
       </c>
-      <c r="BE18">
+      <c r="BF18">
         <v>0.9944750786374379</v>
       </c>
-      <c r="BF18">
+      <c r="BG18">
+        <v>0.9914693431475509</v>
+      </c>
+      <c r="BH18">
+        <v>0.9464334970444814</v>
+      </c>
+      <c r="BI18">
+        <v>0.8857781737701302</v>
+      </c>
+      <c r="BJ18">
+        <v>0.6830425692026182</v>
+      </c>
+      <c r="BK18">
+        <v>0.08696728074618967</v>
+      </c>
+      <c r="BL18">
+        <v>0.01868898448916305</v>
+      </c>
+      <c r="BM18">
         <v>0.974117766191425</v>
       </c>
-      <c r="BG18">
+      <c r="BN18">
         <v>0.6137607525918191</v>
       </c>
     </row>
-    <row r="19" spans="1:59">
+    <row r="19" spans="1:66">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>0.9350988597111926</v>
@@ -3988,45 +4387,66 @@
         <v>0.235614241521993</v>
       </c>
       <c r="AV19">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW19">
         <v>0.993584489501216</v>
       </c>
-      <c r="AW19">
+      <c r="AX19">
         <v>0.9581470031832434</v>
       </c>
-      <c r="AX19">
+      <c r="AY19">
         <v>0.9057199498250654</v>
       </c>
-      <c r="AY19">
+      <c r="AZ19">
         <v>0.7349969737330807</v>
       </c>
-      <c r="AZ19">
+      <c r="BA19">
         <v>0.1155089283074334</v>
       </c>
-      <c r="BA19">
+      <c r="BB19">
         <v>0.02654588568242861</v>
       </c>
-      <c r="BB19">
+      <c r="BC19">
         <v>1</v>
       </c>
-      <c r="BC19">
+      <c r="BD19">
         <v>0.9997999950505075</v>
       </c>
-      <c r="BD19">
+      <c r="BE19">
         <v>0.9854559311109895</v>
       </c>
-      <c r="BE19">
+      <c r="BF19">
         <v>0.994920595121548</v>
       </c>
-      <c r="BF19">
+      <c r="BG19">
+        <v>0.991603354348142</v>
+      </c>
+      <c r="BH19">
+        <v>0.9481955743298468</v>
+      </c>
+      <c r="BI19">
+        <v>0.8880501084940781</v>
+      </c>
+      <c r="BJ19">
+        <v>0.6760232287959481</v>
+      </c>
+      <c r="BK19">
+        <v>0.08124682403607722</v>
+      </c>
+      <c r="BL19">
+        <v>0.02152530674122039</v>
+      </c>
+      <c r="BM19">
         <v>0.9702897169046303</v>
       </c>
-      <c r="BG19">
+      <c r="BN19">
         <v>0.4122460814337736</v>
       </c>
     </row>
-    <row r="20" spans="1:59">
+    <row r="20" spans="1:66">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B20">
         <v>0.943842509940042</v>
@@ -4167,45 +4587,66 @@
         <v>0.2626384887169756</v>
       </c>
       <c r="AV20">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW20">
         <v>0.994989220477803</v>
       </c>
-      <c r="AW20">
+      <c r="AX20">
         <v>0.9752983376953327</v>
       </c>
-      <c r="AX20">
+      <c r="AY20">
         <v>0.9280901110532338</v>
       </c>
-      <c r="AY20">
+      <c r="AZ20">
         <v>0.7534551757053272</v>
       </c>
-      <c r="AZ20">
+      <c r="BA20">
         <v>0.1544528178266525</v>
       </c>
-      <c r="BA20">
+      <c r="BB20">
         <v>0.06429786448837561</v>
-      </c>
-      <c r="BB20">
-        <v>1</v>
       </c>
       <c r="BC20">
         <v>1</v>
       </c>
       <c r="BD20">
+        <v>1</v>
+      </c>
+      <c r="BE20">
         <v>0.9874298445061281</v>
       </c>
-      <c r="BE20">
+      <c r="BF20">
         <v>0.9956641236506755</v>
       </c>
-      <c r="BF20">
+      <c r="BG20">
+        <v>0.9945127411435221</v>
+      </c>
+      <c r="BH20">
+        <v>0.9633567136117311</v>
+      </c>
+      <c r="BI20">
+        <v>0.9085258134377218</v>
+      </c>
+      <c r="BJ20">
+        <v>0.6744159969450421</v>
+      </c>
+      <c r="BK20">
+        <v>0.115974631917495</v>
+      </c>
+      <c r="BL20">
+        <v>0.05531748575464013</v>
+      </c>
+      <c r="BM20">
         <v>0.968987630900756</v>
       </c>
-      <c r="BG20">
+      <c r="BN20">
         <v>0.3172772100005139</v>
       </c>
     </row>
-    <row r="21" spans="1:59">
+    <row r="21" spans="1:66">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B21">
         <v>0.9424729210205292</v>
@@ -4346,45 +4787,66 @@
         <v>0.3541960748912891</v>
       </c>
       <c r="AV21">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW21">
         <v>0.9951878179543077</v>
       </c>
-      <c r="AW21">
+      <c r="AX21">
         <v>0.9715411885462081</v>
       </c>
-      <c r="AX21">
+      <c r="AY21">
         <v>0.9185369531515312</v>
       </c>
-      <c r="AY21">
+      <c r="AZ21">
         <v>0.7459094404264976</v>
       </c>
-      <c r="AZ21">
+      <c r="BA21">
         <v>0.214731601928251</v>
       </c>
-      <c r="BA21">
+      <c r="BB21">
         <v>0.1293472531068167</v>
       </c>
-      <c r="BB21">
+      <c r="BC21">
         <v>1</v>
       </c>
-      <c r="BC21">
+      <c r="BD21">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD21">
+      <c r="BE21">
         <v>0.9842558978080567</v>
       </c>
-      <c r="BE21">
+      <c r="BF21">
         <v>0.9946258798284054</v>
       </c>
-      <c r="BF21">
+      <c r="BG21">
+        <v>0.9951841874316938</v>
+      </c>
+      <c r="BH21">
+        <v>0.9600857355652052</v>
+      </c>
+      <c r="BI21">
+        <v>0.8995182755634746</v>
+      </c>
+      <c r="BJ21">
+        <v>0.6877154090945778</v>
+      </c>
+      <c r="BK21">
+        <v>0.1585444262462216</v>
+      </c>
+      <c r="BL21">
+        <v>0.1137845180768132</v>
+      </c>
+      <c r="BM21">
         <v>0.9726240541574614</v>
       </c>
-      <c r="BG21">
+      <c r="BN21">
         <v>0.3981321517534917</v>
       </c>
     </row>
-    <row r="22" spans="1:59">
+    <row r="22" spans="1:66">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>0.9428971260488295</v>
@@ -4525,45 +4987,66 @@
         <v>0.2510985617422132</v>
       </c>
       <c r="AV22">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW22">
         <v>0.9941885550121877</v>
       </c>
-      <c r="AW22">
+      <c r="AX22">
         <v>0.968392084054653</v>
       </c>
-      <c r="AX22">
+      <c r="AY22">
         <v>0.9157833103012729</v>
       </c>
-      <c r="AY22">
+      <c r="AZ22">
         <v>0.748361899325597</v>
       </c>
-      <c r="AZ22">
+      <c r="BA22">
         <v>0.1208723794332226</v>
       </c>
-      <c r="BA22">
+      <c r="BB22">
         <v>0.02398936881018977</v>
       </c>
-      <c r="BB22">
+      <c r="BC22">
         <v>1</v>
       </c>
-      <c r="BC22">
+      <c r="BD22">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD22">
+      <c r="BE22">
         <v>0.9822739414120091</v>
       </c>
-      <c r="BE22">
+      <c r="BF22">
         <v>0.9944762264855701</v>
       </c>
-      <c r="BF22">
+      <c r="BG22">
+        <v>0.9943801202281477</v>
+      </c>
+      <c r="BH22">
+        <v>0.9589075190577238</v>
+      </c>
+      <c r="BI22">
+        <v>0.8990653192286614</v>
+      </c>
+      <c r="BJ22">
+        <v>0.6896015694245827</v>
+      </c>
+      <c r="BK22">
+        <v>0.08525657146673733</v>
+      </c>
+      <c r="BL22">
+        <v>0.01904636420008394</v>
+      </c>
+      <c r="BM22">
         <v>0.9776371075226237</v>
       </c>
-      <c r="BG22">
+      <c r="BN22">
         <v>0.5345929311112217</v>
       </c>
     </row>
-    <row r="23" spans="1:59">
+    <row r="23" spans="1:66">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B23">
         <v>0.9358584884528106</v>
@@ -4704,45 +5187,66 @@
         <v>0.2104321410348121</v>
       </c>
       <c r="AV23">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW23">
         <v>0.9933878633961351</v>
       </c>
-      <c r="AW23">
+      <c r="AX23">
         <v>0.9607241134695803</v>
       </c>
-      <c r="AX23">
+      <c r="AY23">
         <v>0.9137129097643953</v>
       </c>
-      <c r="AY23">
+      <c r="AZ23">
         <v>0.7458987635257825</v>
       </c>
-      <c r="AZ23">
+      <c r="BA23">
         <v>0.1185627257443962</v>
       </c>
-      <c r="BA23">
+      <c r="BB23">
         <v>0.02238079604172401</v>
       </c>
-      <c r="BB23">
+      <c r="BC23">
         <v>1</v>
       </c>
-      <c r="BC23">
+      <c r="BD23">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD23">
+      <c r="BE23">
         <v>0.9866358551969622</v>
       </c>
-      <c r="BE23">
+      <c r="BF23">
         <v>0.9946213570275182</v>
       </c>
-      <c r="BF23">
+      <c r="BG23">
+        <v>0.9914706967960417</v>
+      </c>
+      <c r="BH23">
+        <v>0.9514731711330778</v>
+      </c>
+      <c r="BI23">
+        <v>0.8960096133954376</v>
+      </c>
+      <c r="BJ23">
+        <v>0.6808596517141402</v>
+      </c>
+      <c r="BK23">
+        <v>0.07941978801571954</v>
+      </c>
+      <c r="BL23">
+        <v>0.01848243717579944</v>
+      </c>
+      <c r="BM23">
         <v>0.9779311708785223</v>
       </c>
-      <c r="BG23">
+      <c r="BN23">
         <v>0.3743167832960189</v>
       </c>
     </row>
-    <row r="24" spans="1:59">
+    <row r="24" spans="1:66">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>0.9456891679319532</v>
@@ -4883,45 +5387,66 @@
         <v>0.2487214448925658</v>
       </c>
       <c r="AV24">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW24">
         <v>0.9937892775828635</v>
       </c>
-      <c r="AW24">
+      <c r="AX24">
         <v>0.972732397475551</v>
       </c>
-      <c r="AX24">
+      <c r="AY24">
         <v>0.9240935314122009</v>
       </c>
-      <c r="AY24">
+      <c r="AZ24">
         <v>0.7553016131613931</v>
       </c>
-      <c r="AZ24">
+      <c r="BA24">
         <v>0.136761255152724</v>
       </c>
-      <c r="BA24">
+      <c r="BB24">
         <v>0.03903464794932785</v>
       </c>
-      <c r="BB24">
+      <c r="BC24">
         <v>1</v>
       </c>
-      <c r="BC24">
+      <c r="BD24">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD24">
+      <c r="BE24">
         <v>0.9882258444939385</v>
       </c>
-      <c r="BE24">
+      <c r="BF24">
         <v>0.9947663862178321</v>
       </c>
-      <c r="BF24">
+      <c r="BG24">
+        <v>0.9945127411435221</v>
+      </c>
+      <c r="BH24">
+        <v>0.9615579318560857</v>
+      </c>
+      <c r="BI24">
+        <v>0.9086157971217571</v>
+      </c>
+      <c r="BJ24">
+        <v>0.6814793404326468</v>
+      </c>
+      <c r="BK24">
+        <v>0.09659172722922246</v>
+      </c>
+      <c r="BL24">
+        <v>0.03068153185591176</v>
+      </c>
+      <c r="BM24">
         <v>0.9770198034063483</v>
       </c>
-      <c r="BG24">
+      <c r="BN24">
         <v>0.3913916088775783</v>
       </c>
     </row>
-    <row r="25" spans="1:59">
+    <row r="25" spans="1:66">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>0.9428971260488295</v>
@@ -5062,45 +5587,66 @@
         <v>0.2504630060876998</v>
       </c>
       <c r="AV25">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW25">
         <v>0.9941885550121877</v>
       </c>
-      <c r="AW25">
+      <c r="AX25">
         <v>0.9685886271854947</v>
       </c>
-      <c r="AX25">
+      <c r="AY25">
         <v>0.9170866020752138</v>
       </c>
-      <c r="AY25">
+      <c r="AZ25">
         <v>0.7485158454741577</v>
       </c>
-      <c r="AZ25">
+      <c r="BA25">
         <v>0.1219069466418133</v>
       </c>
-      <c r="BA25">
+      <c r="BB25">
         <v>0.0234596954206078</v>
       </c>
-      <c r="BB25">
+      <c r="BC25">
         <v>1</v>
       </c>
-      <c r="BC25">
+      <c r="BD25">
         <v>0.9995999901010151</v>
       </c>
-      <c r="BD25">
+      <c r="BE25">
         <v>0.9830739602049312</v>
       </c>
-      <c r="BE25">
+      <c r="BF25">
         <v>0.9943265959492403</v>
       </c>
-      <c r="BF25">
+      <c r="BG25">
+        <v>0.9943801202281477</v>
+      </c>
+      <c r="BH25">
+        <v>0.9589127505181126</v>
+      </c>
+      <c r="BI25">
+        <v>0.8995794371265589</v>
+      </c>
+      <c r="BJ25">
+        <v>0.689958454636613</v>
+      </c>
+      <c r="BK25">
+        <v>0.08549453420890687</v>
+      </c>
+      <c r="BL25">
+        <v>0.01799030689602236</v>
+      </c>
+      <c r="BM25">
         <v>0.977666488487533</v>
       </c>
-      <c r="BG25">
+      <c r="BN25">
         <v>0.5347628776143755</v>
       </c>
     </row>
-    <row r="26" spans="1:59">
+    <row r="26" spans="1:66">
       <c r="A26" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>0.9453617996174155</v>
@@ -5241,39 +5787,60 @@
         <v>0.2267075833447796</v>
       </c>
       <c r="AV26">
+        <v>0.9994666432833114</v>
+      </c>
+      <c r="AW26">
         <v>0.9937892775828635</v>
       </c>
-      <c r="AW26">
+      <c r="AX26">
         <v>0.9721345073793409</v>
       </c>
-      <c r="AX26">
+      <c r="AY26">
         <v>0.9244246214243893</v>
       </c>
-      <c r="AY26">
+      <c r="AZ26">
         <v>0.7515591095663429</v>
       </c>
-      <c r="AZ26">
+      <c r="BA26">
         <v>0.1206092606643635</v>
       </c>
-      <c r="BA26">
+      <c r="BB26">
         <v>0.02618996065179855</v>
       </c>
-      <c r="BB26">
+      <c r="BC26">
         <v>1</v>
       </c>
-      <c r="BC26">
+      <c r="BD26">
         <v>0.9993999851515227</v>
       </c>
-      <c r="BD26">
+      <c r="BE26">
         <v>0.9874238158142211</v>
       </c>
-      <c r="BE26">
+      <c r="BF26">
         <v>0.9946236069386468</v>
       </c>
-      <c r="BF26">
+      <c r="BG26">
+        <v>0.9946467523441129</v>
+      </c>
+      <c r="BH26">
+        <v>0.962028262368767</v>
+      </c>
+      <c r="BI26">
+        <v>0.9062907553562378</v>
+      </c>
+      <c r="BJ26">
+        <v>0.6803365772971084</v>
+      </c>
+      <c r="BK26">
+        <v>0.08124438061865892</v>
+      </c>
+      <c r="BL26">
+        <v>0.01899125654136917</v>
+      </c>
+      <c r="BM26">
         <v>0.9768735099826468</v>
       </c>
-      <c r="BG26">
+      <c r="BN26">
         <v>0.3921049650827302</v>
       </c>
     </row>

</xml_diff>